<commit_message>
sigo con memoria y proy nuevo
</commit_message>
<xml_diff>
--- a/Proyectos/00-000_COSMOBOLITA_SUM/01_Hojas de calculo/DP - Analisis de cargas.xlsx
+++ b/Proyectos/00-000_COSMOBOLITA_SUM/01_Hojas de calculo/DP - Analisis de cargas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andres\Sigma\Proyectos\00-000_COSMOBOLITA_SUM\01_Hojas de calculo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8396C0E-DAF1-486A-BABA-2514FF82D303}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D19F6F8-9D28-48D5-A1D0-EDF73D52E7E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{5EF5C615-0969-4B44-9BD4-17AD9F6ECA56}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{5EF5C615-0969-4B44-9BD4-17AD9F6ECA56}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="65">
   <si>
     <t>Designación</t>
   </si>
@@ -207,6 +207,79 @@
   </si>
   <si>
     <t>2 C 100 x 45 x 10 x 2.00 mm</t>
+  </si>
+  <si>
+    <r>
+      <t>q</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>q</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>y</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>y</t>
+    </r>
+  </si>
+  <si>
+    <t>alfa</t>
+  </si>
+  <si>
+    <t>rad</t>
+  </si>
+  <si>
+    <t>ELU 3 - 0,9 D + 1.6 W</t>
   </si>
 </sst>
 </file>
@@ -217,7 +290,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -239,6 +312,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -390,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -506,6 +587,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,47 +623,59 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -911,7 +1007,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="56" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -928,7 +1024,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="55"/>
+      <c r="A4" s="56"/>
       <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
@@ -950,13 +1046,13 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="62"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -1007,12 +1103,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="58"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
       <c r="E10" s="8">
         <f>SUM(E7:E9)</f>
         <v>28.5</v>
@@ -1028,9 +1124,9 @@
       <c r="A12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="62"/>
-      <c r="C12" s="62"/>
-      <c r="D12" s="62"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
       <c r="E12" s="8">
         <v>51</v>
       </c>
@@ -1039,9 +1135,9 @@
       <c r="A13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="65"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="66"/>
       <c r="E13" s="17">
         <v>-74</v>
       </c>
@@ -1158,8 +1254,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:E34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,27 +1274,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="H1" s="70" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="H1" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="N1" s="70" t="s">
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="N1" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
@@ -1215,13 +1311,13 @@
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -1245,28 +1341,28 @@
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="74"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="73"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
@@ -1288,7 +1384,7 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="54" t="s">
@@ -1297,22 +1393,22 @@
       <c r="C7" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="69"/>
+      <c r="E7" s="68"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="69"/>
+      <c r="J7" s="68"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
-      <c r="N7" s="76" t="s">
+      <c r="N7" s="78" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="54" t="s">
@@ -1326,7 +1422,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
@@ -1341,7 +1437,7 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="77"/>
+      <c r="H8" s="79"/>
       <c r="I8" s="29" t="s">
         <v>28</v>
       </c>
@@ -1350,7 +1446,7 @@
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
-      <c r="N8" s="77"/>
+      <c r="N8" s="79"/>
       <c r="O8" s="29" t="s">
         <v>23</v>
       </c>
@@ -1380,20 +1476,20 @@
       <c r="Q9" s="23"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
-      <c r="H10" s="71" t="s">
+      <c r="H10" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="N10" s="47" t="s">
@@ -1460,19 +1556,19 @@
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
-      <c r="N12" s="72" t="s">
+      <c r="N12" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="74"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="73"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1503,24 +1599,24 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
       <c r="E14" s="33">
         <f>SUM(E11:E13)</f>
         <v>0.81</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="N14" s="78" t="s">
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="N14" s="76" t="s">
         <v>32</v>
       </c>
       <c r="O14" s="53" t="s">
@@ -1544,7 +1640,7 @@
       <c r="J15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="79"/>
+      <c r="N15" s="77"/>
       <c r="O15" s="29" t="s">
         <v>24</v>
       </c>
@@ -1553,8 +1649,8 @@
       <c r="A16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="25" t="s">
         <v>12</v>
       </c>
@@ -1578,8 +1674,8 @@
       <c r="A17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="33">
         <v>1</v>
       </c>
@@ -1588,18 +1684,18 @@
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="72" t="s">
+      <c r="H17" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="73"/>
-      <c r="J17" s="74"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="25" t="s">
         <v>12</v>
       </c>
@@ -1621,25 +1717,25 @@
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="75" t="s">
+      <c r="H19" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="69" t="s">
+      <c r="I19" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="69"/>
+      <c r="J19" s="68"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="75"/>
+      <c r="H20" s="74"/>
       <c r="I20" s="29" t="s">
         <v>28</v>
       </c>
@@ -1667,23 +1763,23 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+      <c r="A22" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
+      <c r="B22" s="67"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E22" s="69"/>
+      <c r="E22" s="68"/>
       <c r="H22" s="45" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
+      <c r="A23" s="67"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="29" t="s">
         <v>28</v>
       </c>
@@ -1692,11 +1788,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="52" t="s">
         <v>12</v>
       </c>
@@ -1706,11 +1802,11 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
       <c r="D25" s="26">
         <f>1.6*$D$17</f>
         <v>1.6</v>
@@ -1721,11 +1817,11 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="66"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="52" t="s">
         <v>12</v>
       </c>
@@ -1735,13 +1831,13 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
@@ -1751,20 +1847,20 @@
       <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69" t="s">
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="69"/>
+      <c r="E30" s="68"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
       <c r="D31" s="29" t="s">
         <v>28</v>
       </c>
@@ -1773,11 +1869,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
       <c r="D32" s="52" t="s">
         <v>12</v>
       </c>
@@ -1787,11 +1883,11 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="26">
         <f>$D$17</f>
         <v>1</v>
@@ -1802,11 +1898,11 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="52" t="s">
         <v>12</v>
       </c>
@@ -1817,33 +1913,6 @@
     </row>
   </sheetData>
   <mergeCells count="37">
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:J7"/>
     <mergeCell ref="N7:N8"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="H10:J10"/>
@@ -1854,6 +1923,33 @@
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="H5:J5"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A22:C23"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1865,8 +1961,8 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,27 +1981,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="H1" s="70" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="H1" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="N1" s="70" t="s">
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="N1" s="80" t="s">
         <v>51</v>
       </c>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
     </row>
     <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
@@ -1922,13 +2018,13 @@
       <c r="L2" s="21"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -1952,28 +2048,28 @@
       <c r="L4" s="21"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
-      <c r="H5" s="67" t="s">
+      <c r="H5" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
       <c r="K5" s="21"/>
       <c r="L5" s="21"/>
-      <c r="N5" s="72" t="s">
+      <c r="N5" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="74"/>
+      <c r="O5" s="72"/>
+      <c r="P5" s="72"/>
+      <c r="Q5" s="73"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="21"/>
@@ -1995,7 +2091,7 @@
       <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="27" t="s">
@@ -2004,22 +2100,22 @@
       <c r="C7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="69" t="s">
+      <c r="D7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="69"/>
+      <c r="E7" s="68"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
-      <c r="H7" s="76" t="s">
+      <c r="H7" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="69"/>
+      <c r="J7" s="68"/>
       <c r="K7" s="21"/>
       <c r="L7" s="21"/>
-      <c r="N7" s="76" t="s">
+      <c r="N7" s="78" t="s">
         <v>0</v>
       </c>
       <c r="O7" s="43" t="s">
@@ -2033,7 +2129,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="68"/>
+      <c r="A8" s="67"/>
       <c r="B8" s="29" t="s">
         <v>23</v>
       </c>
@@ -2048,7 +2144,7 @@
       </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
-      <c r="H8" s="77"/>
+      <c r="H8" s="79"/>
       <c r="I8" s="29" t="s">
         <v>28</v>
       </c>
@@ -2057,7 +2153,7 @@
       </c>
       <c r="K8" s="21"/>
       <c r="L8" s="21"/>
-      <c r="N8" s="77"/>
+      <c r="N8" s="79"/>
       <c r="O8" s="29" t="s">
         <v>23</v>
       </c>
@@ -2087,20 +2183,20 @@
       <c r="Q9" s="23"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="71" t="s">
+      <c r="A10" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
-      <c r="H10" s="71" t="s">
+      <c r="H10" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="71"/>
-      <c r="J10" s="71"/>
+      <c r="I10" s="75"/>
+      <c r="J10" s="75"/>
       <c r="K10" s="21"/>
       <c r="L10" s="21"/>
       <c r="N10" s="47" t="s">
@@ -2167,19 +2263,19 @@
       </c>
       <c r="F12" s="21"/>
       <c r="G12" s="21"/>
-      <c r="H12" s="71" t="s">
+      <c r="H12" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
-      <c r="N12" s="72" t="s">
+      <c r="N12" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="O12" s="73"/>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="74"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="73"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -2210,24 +2306,24 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
       <c r="E14" s="33">
         <f>SUM(E11:E13)</f>
         <v>0.245</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="21"/>
-      <c r="H14" s="71" t="s">
+      <c r="H14" s="75" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="N14" s="78" t="s">
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="N14" s="76" t="s">
         <v>32</v>
       </c>
       <c r="O14" s="36" t="s">
@@ -2251,7 +2347,7 @@
       <c r="J15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="79"/>
+      <c r="N15" s="77"/>
       <c r="O15" s="29" t="s">
         <v>24</v>
       </c>
@@ -2260,8 +2356,8 @@
       <c r="A16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="63"/>
       <c r="D16" s="25" t="s">
         <v>12</v>
       </c>
@@ -2285,8 +2381,8 @@
       <c r="A17" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
+      <c r="B17" s="63"/>
+      <c r="C17" s="63"/>
       <c r="D17" s="33">
         <v>1</v>
       </c>
@@ -2295,18 +2391,18 @@
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21"/>
-      <c r="H17" s="72" t="s">
+      <c r="H17" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="73"/>
-      <c r="J17" s="74"/>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="62"/>
-      <c r="C18" s="62"/>
+      <c r="B18" s="63"/>
+      <c r="C18" s="63"/>
       <c r="D18" s="25" t="s">
         <v>12</v>
       </c>
@@ -2328,25 +2424,25 @@
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
       <c r="G19" s="21"/>
-      <c r="H19" s="75" t="s">
+      <c r="H19" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="69" t="s">
+      <c r="I19" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="J19" s="69"/>
+      <c r="J19" s="68"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="67" t="s">
+      <c r="A20" s="70" t="s">
         <v>33</v>
       </c>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
+      <c r="B20" s="70"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="70"/>
       <c r="F20" s="21"/>
       <c r="G20" s="21"/>
-      <c r="H20" s="75"/>
+      <c r="H20" s="74"/>
       <c r="I20" s="29" t="s">
         <v>28</v>
       </c>
@@ -2373,82 +2469,121 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="68" t="s">
+    <row r="22" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="A22" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B22" s="68"/>
-      <c r="C22" s="68"/>
-      <c r="D22" s="69" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="69"/>
+      <c r="B22" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="55" t="s">
+        <v>61</v>
+      </c>
       <c r="H22" s="45" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
-      <c r="B23" s="68"/>
-      <c r="C23" s="68"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>28</v>
+      </c>
       <c r="D23" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="29" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="66"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" s="26">
-        <f>1.2*$E$14+1.6*$E$16</f>
-        <v>1.254</v>
+      <c r="B24" s="81">
+        <f>ROUND((1.2*E14+1.6*E16)*SIN(H25),2)</f>
+        <v>0.62</v>
+      </c>
+      <c r="C24" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="D24" s="83">
+        <f>ROUND((1.2*E14+1.6*E16)*COS(H25),2)</f>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E24" s="84" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="1">
+        <v>29.5</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="66"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="26">
-        <f>1.6*$D$17</f>
-        <v>1.6</v>
-      </c>
-      <c r="E25" s="26">
-        <f>1.2*$E$14</f>
-        <v>0.29399999999999998</v>
+      <c r="B25" s="81">
+        <f>ROUND(1.2*E14*SIN(H25),2)</f>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="C25" s="81">
+        <f>ROUND(D17*1.6*SIN(H25),2)</f>
+        <v>0.79</v>
+      </c>
+      <c r="D25" s="83">
+        <f>ROUND(1.2*E14*COS(H25),2)</f>
+        <v>0.26</v>
+      </c>
+      <c r="E25" s="83">
+        <f>ROUND(D17*1.6*COS(H25),2)</f>
+        <v>1.39</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="1">
+        <f>RADIANS(H24)</f>
+        <v>0.51487212933832727</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="66" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" s="66"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="26">
-        <f>1.2*$E$14+1.6*$E$18</f>
-        <v>-0.63559999999999994</v>
+      <c r="A26" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="81">
+        <f>ROUND(0.9*E14*SIN(H25),2)</f>
+        <v>0.11</v>
+      </c>
+      <c r="C26" s="82" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="83">
+        <f>ROUND(0.9*E14*COS(H25)+1.5*E18,2)</f>
+        <v>-0.68</v>
+      </c>
+      <c r="E26" s="84" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="67" t="s">
+      <c r="A28" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
+      <c r="B28" s="70"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="70"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="21"/>
@@ -2458,20 +2593,20 @@
       <c r="E29" s="22"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="69" t="s">
+      <c r="B30" s="67"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="69"/>
+      <c r="E30" s="68"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="68"/>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
+      <c r="A31" s="67"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
       <c r="D31" s="29" t="s">
         <v>28</v>
       </c>
@@ -2480,11 +2615,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="66"/>
-      <c r="C32" s="66"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
       <c r="D32" s="16" t="s">
         <v>12</v>
       </c>
@@ -2494,11 +2629,11 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="66"/>
-      <c r="C33" s="66"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
       <c r="D33" s="26">
         <f>$D$17</f>
         <v>1</v>
@@ -2509,11 +2644,11 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="16" t="s">
         <v>12</v>
       </c>
@@ -2523,12 +2658,27 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="N1:R1"/>
+  <mergeCells count="33">
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A30:C31"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A7:A8"/>
     <mergeCell ref="H17:J17"/>
     <mergeCell ref="I19:J19"/>
     <mergeCell ref="H19:H20"/>
@@ -2537,30 +2687,11 @@
     <mergeCell ref="H12:J12"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A30:C31"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A22:C23"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="N1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>